<commit_message>
add usage instructions to sample Excel file
</commit_message>
<xml_diff>
--- a/tests/collateral/content-moderation-excel.xlsx
+++ b/tests/collateral/content-moderation-excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9e9102e27ff69a8/BYODA/Engineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9e9102e27ff69a8/BYODA/Engineering/moderation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{DB481185-3E56-4106-9F59-845E40AE14BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01E36A70-A992-4E9E-AC8F-3FB83228DD7C}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{DB481185-3E56-4106-9F59-845E40AE14BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE120996-5CC0-46FB-9C2F-46E67A59344D}"/>
   <bookViews>
     <workbookView xWindow="19740" yWindow="3645" windowWidth="26985" windowHeight="15345" xr2:uid="{DA791A6E-E96D-4DB0-BBAF-018A8760F67A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Reddit</t>
   </si>
@@ -58,30 +58,12 @@
     <t>alt-right</t>
   </si>
   <si>
-    <t>facist</t>
-  </si>
-  <si>
-    <t>racism</t>
-  </si>
-  <si>
     <t>conspiracy</t>
   </si>
   <si>
-    <t>finance-bro</t>
-  </si>
-  <si>
-    <t>disinformation-ukraine</t>
-  </si>
-  <si>
     <t>disinformation</t>
   </si>
   <si>
-    <t>medical-disinformation</t>
-  </si>
-  <si>
-    <t>gun-rights</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -97,63 +79,9 @@
     <t>intentionally spreading false information</t>
   </si>
   <si>
-    <t>spreading misinformation about the war in ukraine</t>
-  </si>
-  <si>
-    <t>people giving questionable financial advice, including crypto</t>
-  </si>
-  <si>
-    <t>people that refuse to consider that killing someone is a lot easier when you have a gun</t>
-  </si>
-  <si>
-    <t>including the impact of covid, denying vaccins work, and/or promote alternative treatments over science-based treatments</t>
-  </si>
-  <si>
-    <t>Hatred of, contempt for, or prejudice against women</t>
-  </si>
-  <si>
-    <t>prejudiced belief that one race is superior to others</t>
-  </si>
-  <si>
-    <t>gambling</t>
-  </si>
-  <si>
-    <t>nazi</t>
-  </si>
-  <si>
-    <t>likes hitler, facism, racism and all that</t>
-  </si>
-  <si>
-    <t>disinformation-war</t>
-  </si>
-  <si>
     <t>Twitter</t>
   </si>
   <si>
-    <t>troll</t>
-  </si>
-  <si>
-    <t>bot</t>
-  </si>
-  <si>
-    <t>impersonater</t>
-  </si>
-  <si>
-    <t>tries to appear as someone they are not</t>
-  </si>
-  <si>
-    <t>posts deliberately offensive or provocative messages</t>
-  </si>
-  <si>
-    <t>likely an automated account, trying to appear to not be an automated account</t>
-  </si>
-  <si>
-    <t>ufo</t>
-  </si>
-  <si>
-    <t>misogyny</t>
-  </si>
-  <si>
     <t>Odysee</t>
   </si>
   <si>
@@ -244,19 +172,25 @@
     <t>Web</t>
   </si>
   <si>
-    <t>To get started, add entries to the table in the 'moderation' sheet</t>
-  </si>
-  <si>
     <t>Pretty much all columns in the table are optional but you need to enter a value for 'category' to have the entry included in the resulting YAML file</t>
   </si>
   <si>
-    <t>You can use this Excel sheet to collect inforation about social media accounts you consider people may want to block</t>
-  </si>
-  <si>
     <t>Once you are done, you can either email to excel sheet to steven+byomod@byoda.org and I'll generate a YAML file and publish it under https://byomod.org/lists</t>
   </si>
   <si>
     <t xml:space="preserve">Alternatively, if you are good with Github, Python and have access to a webserver, you can follow the instructions on </t>
+  </si>
+  <si>
+    <t>You can use this Excel sheet to collect information about social media accounts you think people may want to block</t>
+  </si>
+  <si>
+    <t>To get started:</t>
+  </si>
+  <si>
+    <t>In the moderation sheet you can add data about accounts. You can use one line per person and then use the various columns to document the various social media accounts of that person</t>
+  </si>
+  <si>
+    <t>You can define what categories you want to use to in the 'categories' sheet. You can see some example entries in this sheet and you can replace them or add additional categories</t>
   </si>
 </sst>
 </file>
@@ -339,6 +273,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35074C6F-0268-4702-84C3-B066C5A866AD}" name="Table1" displayName="Table1" ref="A1:AJ281" totalsRowShown="0">
   <autoFilter ref="A1:AJ281" xr:uid="{35074C6F-0268-4702-84C3-B066C5A866AD}"/>
@@ -385,8 +323,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90DACF00-DB4C-4DC3-890D-F0E20718FDE6}" name="Table2" displayName="Table2" ref="A1:B18" totalsRowShown="0">
-  <autoFilter ref="A1:B18" xr:uid="{90DACF00-DB4C-4DC3-890D-F0E20718FDE6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{90DACF00-DB4C-4DC3-890D-F0E20718FDE6}" name="Table2" displayName="Table2" ref="A1:B38" totalsRowShown="0">
+  <autoFilter ref="A1:B38" xr:uid="{90DACF00-DB4C-4DC3-890D-F0E20718FDE6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FF7B92BC-51F2-483D-A3BA-D6330B748284}" name="Category"/>
     <tableColumn id="2" xr3:uid="{5F4213D1-DE26-4B92-8304-D975EA58EBDC}" name="Description"/>
@@ -712,37 +650,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06C7272-2CA7-48C5-860F-C49E1B1CE290}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -755,7 +703,7 @@
   <dimension ref="A1:AJ189"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,58 +728,58 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
       <c r="J1" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="M1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="O1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="Q1" t="s">
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="S1" t="s">
         <v>1</v>
@@ -846,46 +794,46 @@
         <v>4</v>
       </c>
       <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" t="s">
         <v>40</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AH1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>65</v>
-      </c>
       <c r="AI1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="AJ1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1653,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17EC9E53-7A32-4939-8EA1-038A5E101876}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,10 +1615,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1678,123 +1626,23 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>